<commit_message>
Pushing updates using CMD script
</commit_message>
<xml_diff>
--- a/TESIS_MAESTRIA/Planificacion.xlsx
+++ b/TESIS_MAESTRIA/Planificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\research_papers\TESIS_MAESTRIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CB59BDF-A036-44A2-9B79-0AAD177C2E69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F44F92F-F102-4716-980C-70D00FEA053D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{51EFCB27-CC9C-40E5-B3B2-B7356EC018C9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>SEMANA 1</t>
   </si>
@@ -63,16 +63,22 @@
     <t>Obtener informacion sobre los lineamientos en la categorizacion de seguridad de los proyectos de software en ejecucion.</t>
   </si>
   <si>
-    <t>Identificar metodologia existente para categorizar el nivel de seguridad en la organizacion</t>
-  </si>
-  <si>
-    <t>Identificar metodologia existente para seleccionar los controles de seguridad</t>
-  </si>
-  <si>
-    <t>Identificar procedimientos y herramientas para dar el seguimiento de las implementaciones de los controles de seguridad</t>
-  </si>
-  <si>
     <t>ACTIVIDADES PROGRAMADAS PARA TESIS II</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Identificar metodologia existente para categorizar el nivel de seguridad en la organización.</t>
+  </si>
+  <si>
+    <t>Identificar metodologia existente para seleccionar los controles de seguridad.</t>
+  </si>
+  <si>
+    <t>Identificar procedimientos y herramientas para dar el seguimiento de las implementaciones de los controles de seguridad.</t>
+  </si>
+  <si>
+    <t>Establecer formatos de encuestas para que los arquitectos de software puedan completar.</t>
   </si>
 </sst>
 </file>
@@ -294,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -305,6 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -314,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,7 +639,7 @@
   <dimension ref="B1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,16 +653,16 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -686,7 +693,9 @@
         <v>7</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -698,7 +707,9 @@
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -711,7 +722,9 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -719,47 +732,57 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
     </row>
@@ -784,7 +807,7 @@
       <c r="I12" s="9"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
+      <c r="B15" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>